<commit_message>
+bug fixes +error handling
</commit_message>
<xml_diff>
--- a/app/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/app/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -686,7 +686,7 @@
   <dimension ref="B2:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,7 +762,7 @@
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="12">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E8" s="6"/>
     </row>
@@ -772,7 +772,7 @@
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="12">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E9" s="6"/>
     </row>

</xml_diff>